<commit_message>
More testcases and Script Added
</commit_message>
<xml_diff>
--- a/Documentation/Verification_Plan/Functional_Test_Plan_Template.xlsx
+++ b/Documentation/Verification_Plan/Functional_Test_Plan_Template.xlsx
@@ -18,21 +18,26 @@
     <sheet name="BLK-5" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-1'!$A$4:$J$54</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-1'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-2'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-3'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-4'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-5'!$A$4:$J$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-1'!$A$4:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-1'!$A$4:$J$54</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'BLK-1'!$A$4:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'BLK-1'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-2'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'BLK-2'!$A$4:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'BLK-2'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-3'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'BLK-3'!$A$4:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'BLK-3'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-4'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0" vbProcedure="false">'BLK-4'!$A$4:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'BLK-4'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">'BLK-5'!$A$4:$J$4</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">'BLK-5'!$A$4:$J$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'BLK-5'!$A$4:$J$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -44,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="79">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -1579,11 +1584,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="25712071"/>
-        <c:axId val="34219932"/>
+        <c:axId val="56163683"/>
+        <c:axId val="83647886"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="25712071"/>
+        <c:axId val="56163683"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,14 +1624,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34219932"/>
+        <c:crossAx val="83647886"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34219932"/>
+        <c:axId val="83647886"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1669,7 +1674,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25712071"/>
+        <c:crossAx val="56163683"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1717,9 +1722,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>704160</xdr:colOff>
+      <xdr:colOff>703800</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>8280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1729,7 +1734,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1039320" y="2209680"/>
-          <a:ext cx="4650120" cy="1113480"/>
+          <a:ext cx="4650480" cy="1113120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2072,9 +2077,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>599040</xdr:colOff>
+      <xdr:colOff>598680</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2083,7 +2088,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="657000" y="193320"/>
-        <a:ext cx="5123520" cy="2581920"/>
+        <a:ext cx="5123160" cy="2581560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2529,14 +2534,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="43.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="30" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="50.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="29" width="16.45"/>
@@ -2545,15 +2550,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="9.18"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="30" min="23" style="6" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="6" width="9.18"/>
@@ -2961,7 +2966,9 @@
         <v>55</v>
       </c>
       <c r="D10" s="43"/>
-      <c r="E10" s="44"/>
+      <c r="E10" s="44" t="s">
+        <v>44</v>
+      </c>
       <c r="F10" s="45"/>
       <c r="G10" s="46"/>
       <c r="H10" s="43"/>
@@ -2990,7 +2997,9 @@
         <v>55</v>
       </c>
       <c r="D11" s="43"/>
-      <c r="E11" s="44"/>
+      <c r="E11" s="44" t="s">
+        <v>44</v>
+      </c>
       <c r="F11" s="45"/>
       <c r="G11" s="46"/>
       <c r="H11" s="43"/>
@@ -3019,7 +3028,9 @@
         <v>58</v>
       </c>
       <c r="D12" s="43"/>
-      <c r="E12" s="44"/>
+      <c r="E12" s="44" t="s">
+        <v>44</v>
+      </c>
       <c r="F12" s="45"/>
       <c r="G12" s="46"/>
       <c r="H12" s="43"/>
@@ -3048,7 +3059,9 @@
         <v>58</v>
       </c>
       <c r="D13" s="43"/>
-      <c r="E13" s="44"/>
+      <c r="E13" s="44" t="s">
+        <v>44</v>
+      </c>
       <c r="F13" s="45"/>
       <c r="G13" s="46"/>
       <c r="H13" s="43"/>
@@ -3077,7 +3090,9 @@
         <v>58</v>
       </c>
       <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
+      <c r="E14" s="44" t="s">
+        <v>44</v>
+      </c>
       <c r="F14" s="45"/>
       <c r="G14" s="46"/>
       <c r="H14" s="43"/>
@@ -3106,7 +3121,9 @@
         <v>58</v>
       </c>
       <c r="D15" s="43"/>
-      <c r="E15" s="44"/>
+      <c r="E15" s="44" t="s">
+        <v>44</v>
+      </c>
       <c r="F15" s="45"/>
       <c r="G15" s="46"/>
       <c r="H15" s="43"/>
@@ -4147,7 +4164,7 @@
       <c r="U54" s="45"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J54"/>
+  <autoFilter ref="A4:J4"/>
   <mergeCells count="17">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="L1:M1"/>
@@ -4516,12 +4533,12 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F5:F54" type="list">
+      <formula1>"CRITICAL,HIGH,MEDIUM,LOW"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I5:I54" type="list">
       <formula1>"DSGN,TB,TC"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F5:F54" type="list">
-      <formula1>"CRITICAL,HIGH,MEDIUM,LOW"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L5:L54 N5:N54 P5:P54 R5:R54 T5:T54" type="list">
@@ -4565,7 +4582,7 @@
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="50.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="29" width="16.45"/>
@@ -4574,15 +4591,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="9.18"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="30" min="23" style="6" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="6" width="9.18"/>
@@ -6256,7 +6273,7 @@
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="50.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="29" width="16.45"/>
@@ -6265,15 +6282,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="9.18"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="30" min="23" style="6" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="6" width="9.18"/>
@@ -7947,7 +7964,7 @@
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="50.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="29" width="16.45"/>
@@ -7956,15 +7973,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="9.18"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="30" min="23" style="6" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="6" width="9.18"/>
@@ -9638,7 +9655,7 @@
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="30" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="30" width="50.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="29" width="16.45"/>
@@ -9647,15 +9664,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="9.18"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="30" min="23" style="6" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="31" style="6" width="9.18"/>

</xml_diff>